<commit_message>
Identificação de entidades, atributos e definições
1. Identificar entidades.
2. Identificar atributos.
3. Identificar atributos opcionais e mandatórios (obrigatórios).
Identificar a cardinalidade mínima de cada atributo, conforme segue:
a. Cardinalidade mínima
i. Min = 0 – Atributo Opcional (o)
ii. Min = 1 – Mandatório (*)
</commit_message>
<xml_diff>
--- a/CheckPoint1 - Projeto de Streaming de Músicas.xlsx
+++ b/CheckPoint1 - Projeto de Streaming de Músicas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dd74dbd2b7b8037e/Documentos/FIAP/1TSCG/RELATIONAL DATABASE ^0 SQL/CheckPoint/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{175BCE09-CC0C-415C-8124-1839ADEEA202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="191" documentId="8_{B0AE2542-0EFB-40BE-AB6B-D617AC97CAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02B4C2EC-DAF9-47D0-A5B7-3B0CAB168686}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{73A1BEB3-AFF6-417D-973B-9469212A793F}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="60">
   <si>
     <t>Nome do seu Projeto: Sistema de Streaming de Músicas - SSM</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Telefone</t>
   </si>
   <si>
-    <t>nr_telefone</t>
-  </si>
-  <si>
     <t>C, M</t>
   </si>
   <si>
@@ -165,9 +162,6 @@
     <t>T_SSM_ALBUM</t>
   </si>
   <si>
-    <t>Nome do álbum</t>
-  </si>
-  <si>
     <t>Data de lançamento</t>
   </si>
   <si>
@@ -223,13 +217,28 @@
   </si>
   <si>
     <t>Código da playlist</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Mono</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Título do álbum</t>
+  </si>
+  <si>
+    <t>S, D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,16 +262,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -271,11 +313,131 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="hair">
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -285,50 +447,121 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -341,19 +574,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D20E1F32-A66E-4511-94DB-165FC493F831}" name="Tabela4" displayName="Tabela4" ref="B3:G44" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="B3:G44" xr:uid="{B5D24989-C3E2-4ABD-8E33-EFEB0D26C063}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{786D591F-F9DD-4561-B78A-E6A8EFB9598C}" name="Entidades"/>
-    <tableColumn id="2" xr3:uid="{0E61AD9D-ABC0-400D-A2E0-36991F747CB7}" name="Atributos"/>
-    <tableColumn id="3" xr3:uid="{59C1038A-7E9B-4140-8279-371B751B93C3}" name="Nomenclatura e #Chave Primária" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{64C0D8DF-0E47-4A0D-BBC9-61F4E201FB7D}" name="Atributo Simples, Composto, Determinante e/ou Multivalorado" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{0D0B63D8-114F-4F96-882A-815C836CC5C5}" name="Opcional(o) ou Obrigatório(*)" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{571BCD12-5397-4D92-B47C-881501203838}" name="Monovalorado ou Multivalorado" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -656,471 +878,726 @@
   <dimension ref="B1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="1.81640625" customWidth="1"/>
     <col min="2" max="2" width="25.453125" customWidth="1"/>
-    <col min="3" max="3" width="50" style="2" customWidth="1"/>
-    <col min="4" max="4" width="25.453125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.453125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="20.90625" customWidth="1"/>
     <col min="7" max="7" width="21.81640625" customWidth="1"/>
     <col min="8" max="8" width="1.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.35">
       <c r="D2"/>
     </row>
-    <row r="3" spans="2:7" s="4" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="2:7" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="21" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
+      <c r="B4" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C5" t="s">
+      <c r="B5" s="30"/>
+      <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="E5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C6" t="s">
+      <c r="B6" s="30"/>
+      <c r="C6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C7" t="s">
+      <c r="B7" s="30"/>
+      <c r="C7" s="13" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="E7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C8" t="s">
+      <c r="B8" s="30"/>
+      <c r="C8" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="24" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C9" t="s">
+      <c r="B9" s="30"/>
+      <c r="C9" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="E9" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C10" t="s">
+      <c r="B10" s="30"/>
+      <c r="C10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="4"/>
+      <c r="E10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="F10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="G10" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="5" t="s">
+    </row>
+    <row r="11" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="31"/>
+      <c r="C11" s="15" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C11" t="s">
+      <c r="D11" s="7"/>
+      <c r="E11" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B12" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
+      <c r="C12" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" s="8"/>
+      <c r="E12" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B13" s="30"/>
+      <c r="C13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C13" t="s">
+      <c r="D13" s="5"/>
+      <c r="E13" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="31"/>
+      <c r="C14" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C14" t="s">
+      <c r="D14" s="9"/>
+      <c r="E14" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" s="27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B15" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B15" t="s">
+      <c r="C15" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" s="10"/>
+      <c r="E15" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" s="28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="31"/>
+      <c r="C16" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C16" t="s">
+      <c r="D16" s="9"/>
+      <c r="E16" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B17" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B17" t="s">
+      <c r="C17" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" s="10"/>
+      <c r="E17" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="31"/>
+      <c r="C18" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C18" t="s">
+      <c r="D18" s="9"/>
+      <c r="E18" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" s="27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B19" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B19" t="s">
+      <c r="C19" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" s="10"/>
+      <c r="E19" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="30"/>
+      <c r="C20" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-    </row>
-    <row r="20" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C20" t="s">
+      <c r="D20" s="4"/>
+      <c r="E20" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G20" s="24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="30"/>
+      <c r="C21" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-    </row>
-    <row r="21" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C21" t="s">
+      <c r="D21" s="5"/>
+      <c r="E21" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="30"/>
+      <c r="C22" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-    </row>
-    <row r="22" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C22" t="s">
+      <c r="D22" s="4"/>
+      <c r="E22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G22" s="24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="31"/>
+      <c r="C23" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-    </row>
-    <row r="23" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C23" t="s">
+      <c r="D23" s="7"/>
+      <c r="E23" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" s="25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B24" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B24" t="s">
+      <c r="C24" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G24" s="26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B25" s="30"/>
+      <c r="C25" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B26" s="31"/>
+      <c r="C26" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C24" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C25" t="s">
+      <c r="D26" s="9"/>
+      <c r="E26" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B27" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C26" t="s">
+      <c r="C27" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B27" t="s">
+      <c r="D27" s="10"/>
+      <c r="E27" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G27" s="28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B28" s="30"/>
+      <c r="C28" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D28" s="4"/>
+      <c r="E28" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G28" s="24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B29" s="31"/>
+      <c r="C29" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C28" s="2" t="s">
+      <c r="D29" s="7"/>
+      <c r="E29" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G29" s="25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B30" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C29" s="2" t="s">
+      <c r="C30" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B30" t="s">
+      <c r="D30" s="8"/>
+      <c r="E30" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G30" s="26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B31" s="30"/>
+      <c r="C31" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G31" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B32" s="31"/>
+      <c r="C32" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="27"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B33" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C31" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C32" s="2" t="s">
+      <c r="C33" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B33" t="s">
+      <c r="D33" s="10"/>
+      <c r="E33" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G33" s="28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B34" s="30"/>
+      <c r="C34" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G34" s="24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B35" s="30"/>
+      <c r="C35" s="35" t="s">
         <v>46</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C34" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C35" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C36" s="2" t="s">
+      <c r="F35" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G35" s="23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B36" s="31"/>
+      <c r="C36" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G36" s="27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B37" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G37" s="28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B38" s="30"/>
+      <c r="C38" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B37" t="s">
+      <c r="D38" s="4"/>
+      <c r="E38" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G38" s="24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B39" s="30"/>
+      <c r="C39" s="35" t="s">
         <v>50</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C38" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C39" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C40" s="2" t="s">
+      <c r="G39" s="23"/>
+    </row>
+    <row r="40" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B40" s="31"/>
+      <c r="C40" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="27"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B41" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B41" t="s">
+      <c r="D41" s="10"/>
+      <c r="E41" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G41" s="28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B42" s="30"/>
+      <c r="C42" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C42" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G42" s="24" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C43" s="2" t="s">
+      <c r="B43" s="30"/>
+      <c r="C43" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G43" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B44" s="31"/>
+      <c r="C44" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C44" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G44" s="27" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="12">
+    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="B19:B23"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="B33:B36"/>
     <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B4:B11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B18"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>